<commit_message>
all tests complete, all graphs in pp
</commit_message>
<xml_diff>
--- a/testing/ica-v2 effect on population desnity - Air Temperature-spreadsheet.xlsx
+++ b/testing/ica-v2 effect on population desnity - Air Temperature-spreadsheet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\DiseaseSpread\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B2DC2561-1FA0-44BC-96EB-80B045EA6E56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246A5CBE-1019-47A8-A74B-B3BD4FAE5FF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ica-v2 effect on population des" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'ica-v2 effect on population des'!$20:$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'ica-v2 effect on population des'!$AC$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'ica-v2 effect on population des'!$AJ$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'ica-v2 effect on population des'!$H$20</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'ica-v2 effect on population des'!$O$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'ica-v2 effect on population des'!$V$20</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -681,9 +681,28 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Average Time Taken for the Population to Become Infected </a:t>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Air Temperature</a:t>
             </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time Taken (average of 10) to infect whole population </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -731,10 +750,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11151071663745214"/>
-          <c:y val="7.0220111796393439E-2"/>
+          <c:x val="3.3640227072001989E-2"/>
+          <c:y val="0.14054973897493583"/>
           <c:w val="0.81475962379702538"/>
-          <c:h val="0.8416746864975212"/>
+          <c:h val="0.77134504340803556"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -745,7 +764,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>0</c:v>
+            <c:v>Air temperature 0°C</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -803,7 +822,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>10</c:v>
+            <c:v>Air temperature 10°C</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -861,7 +880,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>20</c:v>
+            <c:v>Air temperature 20°C</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -919,7 +938,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>30</c:v>
+            <c:v>Air temperature 30°C</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -977,7 +996,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>40</c:v>
+            <c:v>Air temperature 40°C</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1050,74 +1069,6 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Air</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Temperature (°C)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="7.894605047160632E-3"/>
-              <c:y val="0.41686330403727306"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1267,9 +1218,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.2049006241710948E-2"/>
-          <c:y val="4.5426842475115997E-2"/>
-          <c:w val="6.946259842519685E-2"/>
+          <c:x val="0.87273248965084538"/>
+          <c:y val="0.10403484179862134"/>
+          <c:w val="0.10760330322040716"/>
           <c:h val="0.83970180810731976"/>
         </c:manualLayout>
       </c:layout>
@@ -1899,15 +1850,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
+      <xdr:colOff>276226</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2231,10 +2182,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AG4" workbookViewId="0">
       <selection activeCell="AY24" sqref="AY24"/>
     </sheetView>
   </sheetViews>

</xml_diff>